<commit_message>
Updated dbml star schema.
</commit_message>
<xml_diff>
--- a/datasets/excel-datasets/dataset-car-deals.xlsx
+++ b/datasets/excel-datasets/dataset-car-deals.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcastro/Faculdade/Mestrado/1-ano/semestre-1/TAAD/projeto-2021/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcastro/Faculdade/Mestrado/1-ano/semestre-1/TAAD/projeto-2021/car-deals-etl/datasets/excel-datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2358ECFA-E380-C047-A9A1-4E25C21B0582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6595F398-CC13-3349-BCAE-A66FB4A2EA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="12800" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2634,12 +2634,15 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -2982,17 +2985,21 @@
   <dimension ref="A1:X82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V80" sqref="V80"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="45.1640625" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
     <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" customWidth="1"/>
+    <col min="13" max="13" width="24.5" customWidth="1"/>
+    <col min="16" max="16" width="17.83203125" customWidth="1"/>
+    <col min="17" max="17" width="16.33203125" customWidth="1"/>
     <col min="21" max="21" width="22" customWidth="1"/>
     <col min="22" max="22" width="19.83203125" customWidth="1"/>
     <col min="23" max="23" width="26.83203125" customWidth="1"/>
@@ -5564,7 +5571,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>58</v>
       </c>
@@ -5634,7 +5641,7 @@
       <c r="W36" t="s">
         <v>705</v>
       </c>
-      <c r="X36" t="s">
+      <c r="X36" s="3" t="s">
         <v>756</v>
       </c>
     </row>

</xml_diff>